<commit_message>
changed eeprom structure for VIN.  currently only edits vin via parameters config
</commit_message>
<xml_diff>
--- a/Files/Parameters for Record Sets.xlsx
+++ b/Files/Parameters for Record Sets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herbere\Desktop\Chamber Decompress\Builds\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balzermi\Documents\AGCO Corporation\EDT\Models\BL21\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1792,8 +1792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="C170" sqref="C170"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1840,7 +1840,7 @@
       </c>
       <c r="D2" s="12">
         <f>HEX2DEC(F2)+HEX2DEC($G$2)</f>
-        <v>256</v>
+        <v>288</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>121</v>
@@ -1849,7 +1849,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="11">
-        <v>100</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1864,7 +1864,7 @@
       </c>
       <c r="D3" s="12">
         <f t="shared" ref="D3:D5" si="0">HEX2DEC(F3)+HEX2DEC($G$2)</f>
-        <v>273</v>
+        <v>305</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>121</v>
@@ -1886,7 +1886,7 @@
       </c>
       <c r="D4" s="12">
         <f t="shared" si="0"/>
-        <v>306</v>
+        <v>338</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>121</v>
@@ -1908,7 +1908,7 @@
       </c>
       <c r="D5" s="12">
         <f t="shared" si="0"/>
-        <v>512</v>
+        <v>544</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>122</v>
@@ -10571,11 +10571,11 @@
       </c>
       <c r="D2">
         <f>HEX2DEC(VLOOKUP($A2,StoredParameters!$A$2:$G$315,7,FALSE))</f>
-        <v>256</v>
+        <v>288</v>
       </c>
       <c r="E2">
         <f t="array" ref="E2">VLOOKUP($A2&amp;"""SEGMENT_CHECKSUM""",CHOOSE({1,2},StoredParameters!$A$2:$A$288&amp;StoredParameters!$C$2:$C$288,StoredParameters!$D$2:$D$288),2,FALSE)</f>
-        <v>512</v>
+        <v>544</v>
       </c>
       <c r="G2" t="s">
         <v>392</v>

</xml_diff>